<commit_message>
feat: Add Phase 2A openEHR archetypes and sync README
openEHR Archetypes (Phase 2A):
- blood_glucose_cgm.v0: CGM archetype with TIR, GMI, glycemic variability
- body_composition_wearable.v0: BIA smart scale data, segmental analysis
- exercise_session.v0: Workout tracking, TRIMP/TSS, running/cycling/swimming

README updated: 15 archetypes total (5 CLUSTER + 10 OBSERVATION)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/ConceptMapVendorToLOINC.xlsx
+++ b/output/ConceptMapVendorToLOINC.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
   <si>
     <t>Property</t>
   </si>
@@ -115,18 +115,15 @@
     <t>Copyright</t>
   </si>
   <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>http://loinc.org</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>https://2rdoc.pt/ig/ios-lifestyle-medicine/ValueSet/vendor-codes-vs</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>https://2rdoc.pt/ig/ios-lifestyle-medicine/ValueSet/loinc-observations-vs</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>http://loinc.org</t>
   </si>
   <si>
     <t>HKQuantityTypeIdentifierHeartRateVariabilitySDNN</t>
@@ -504,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -670,14 +664,6 @@
       </c>
       <c r="B20" t="s" s="2">
         <v>33</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -695,206 +681,206 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="E3" t="s" s="2">
         <v>43</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="E4" t="s" s="2">
         <v>47</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="E5" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="E6" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>57</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>58</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="D7" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="E7" t="s" s="2">
         <v>60</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>62</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s" s="2">
         <v>63</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="E8" t="s" s="2">
         <v>64</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>66</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s" s="2">
         <v>67</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="E9" t="s" s="2">
         <v>68</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>70</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>71</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="E10" t="s" s="2">
         <v>72</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s" s="2">
-        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s" s="2">
         <v>75</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="E11" t="s" s="2">
         <v>76</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E11" t="s" s="2">
-        <v>78</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="E12" t="s" s="2">
         <v>80</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="E12" t="s" s="2">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -912,87 +898,87 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="E5" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1010,104 +996,104 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="E5" t="s" s="2">
         <v>95</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="E5" t="s" s="2">
-        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1125,70 +1111,70 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s" s="2">
         <v>47</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="E4" t="s" s="2">
         <v>103</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1206,87 +1192,87 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="E1" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="E3" t="s" s="2">
         <v>108</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s" s="2">
         <v>111</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="D4" t="s" s="2">
         <v>112</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="E4" t="s" s="2">
         <v>113</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="E4" t="s" s="2">
-        <v>115</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>